<commit_message>
updating some of our inventory that was already processed.
</commit_message>
<xml_diff>
--- a/check sample work/pH QAQC/Sampling_Metadata_Feb2018-Oct2019.xlsx
+++ b/check sample work/pH QAQC/Sampling_Metadata_Feb2018-Oct2019.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\915712257\Documents\R\rye-tech-sfsu\2021-season-summary\check sample work\pH QAQC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rye-Tech\Documents\R\rye-tech-home\2021-season-summary\check sample work\pH QAQC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AE89CF-0522-4A25-9F53-8063C717AC08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample metadata" sheetId="3" r:id="rId1"/>
     <sheet name="procs list nov2019 plus" sheetId="5" r:id="rId2"/>
     <sheet name="procs list feb2018 to oct2019" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="149">
   <si>
     <t>B-0061</t>
   </si>
@@ -440,12 +441,45 @@
   </si>
   <si>
     <t>11/10/2020, pH;</t>
+  </si>
+  <si>
+    <t>6/29/19,pH;</t>
+  </si>
+  <si>
+    <t>7/18/18, pH;</t>
+  </si>
+  <si>
+    <t>4/11/19, pH;</t>
+  </si>
+  <si>
+    <t>5/1/19, pH;</t>
+  </si>
+  <si>
+    <t>7/10/19, pH;</t>
+  </si>
+  <si>
+    <t>3/11/19, pH;</t>
+  </si>
+  <si>
+    <t>6/25/19, pH;</t>
+  </si>
+  <si>
+    <t>5/21/19, pH;</t>
+  </si>
+  <si>
+    <t>2/22/19, pH;</t>
+  </si>
+  <si>
+    <t>1/30/19, pH;</t>
+  </si>
+  <si>
+    <t>3/20/19, pH;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
@@ -893,11 +927,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
@@ -3389,7 +3423,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G16463">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G16463">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3397,7 +3431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3456,12 +3490,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3655,7 +3689,7 @@
         <v>16.736034513682998</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3838,6 +3872,9 @@
       <c r="F16" s="20">
         <v>15.1164646148681</v>
       </c>
+      <c r="G16" s="25" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
@@ -3904,6 +3941,9 @@
       <c r="F19" s="20">
         <v>17.5979527697924</v>
       </c>
+      <c r="G19" s="25" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
@@ -4056,6 +4096,9 @@
       <c r="F26" s="20">
         <v>20.8</v>
       </c>
+      <c r="G26" s="25" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
@@ -4122,6 +4165,9 @@
       <c r="F29" s="20">
         <v>13.334194849999999</v>
       </c>
+      <c r="G29" s="25" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
@@ -4142,6 +4188,9 @@
       <c r="F30" s="16">
         <v>12.824123981783</v>
       </c>
+      <c r="G30" s="25" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
@@ -4368,6 +4417,9 @@
       <c r="F41" s="20">
         <v>13.4</v>
       </c>
+      <c r="G41" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="16">
@@ -4408,6 +4460,9 @@
       <c r="F43" s="17">
         <v>12.5652239569302</v>
       </c>
+      <c r="G43" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="16">
@@ -4428,6 +4483,9 @@
       <c r="F44" s="20">
         <v>13.1396989883988</v>
       </c>
+      <c r="G44" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="16">
@@ -4448,6 +4506,9 @@
       <c r="F45" s="20">
         <v>13.333217822885899</v>
       </c>
+      <c r="G45" s="25" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="16">
@@ -4508,6 +4569,9 @@
       <c r="F48" s="17">
         <v>13.15465663</v>
       </c>
+      <c r="G48" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="16">
@@ -4594,6 +4658,9 @@
       <c r="F52" s="17">
         <v>13.0293914751136</v>
       </c>
+      <c r="G52" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="16">
@@ -4614,6 +4681,9 @@
       <c r="F53" s="20">
         <v>13.243272250417</v>
       </c>
+      <c r="G53" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="16">
@@ -4657,6 +4727,9 @@
       <c r="F55" s="20">
         <v>12.981672430854999</v>
       </c>
+      <c r="G55" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
@@ -4720,6 +4793,9 @@
       <c r="F58" s="20">
         <v>14.28838139</v>
       </c>
+      <c r="G58" s="25" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="16">
@@ -4740,6 +4816,9 @@
       <c r="F59" s="20">
         <v>12.5370592775172</v>
       </c>
+      <c r="G59" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="16">
@@ -4760,6 +4839,9 @@
       <c r="F60" s="20">
         <v>16.229541859310199</v>
       </c>
+      <c r="G60" s="25" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="16">
@@ -4780,6 +4862,9 @@
       <c r="F61" s="17">
         <v>13.322875686624</v>
       </c>
+      <c r="G61" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="16">
@@ -4843,6 +4928,9 @@
       <c r="F64" s="20">
         <v>13.1152615644825</v>
       </c>
+      <c r="G64" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="16">
@@ -4909,6 +4997,9 @@
       <c r="F67" s="22">
         <v>15.018599999999999</v>
       </c>
+      <c r="G67" s="25" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="16">
@@ -4992,6 +5083,9 @@
       <c r="F71" s="16">
         <v>13.849871981341</v>
       </c>
+      <c r="G71" s="25" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="16">
@@ -5012,6 +5106,9 @@
       <c r="F72" s="20">
         <v>13.9233166016284</v>
       </c>
+      <c r="G72" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="16">
@@ -5032,6 +5129,9 @@
       <c r="F73" s="20">
         <v>13.916645772569399</v>
       </c>
+      <c r="G73" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="16">
@@ -5172,8 +5272,11 @@
       <c r="F80" s="20">
         <v>12.685515474343401</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="16">
         <v>79</v>
       </c>
@@ -5193,7 +5296,7 @@
         <v>16.360399999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="16">
         <v>80</v>
       </c>
@@ -5213,7 +5316,7 @@
         <v>20.671867840000001</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="16">
         <v>81</v>
       </c>
@@ -5233,7 +5336,7 @@
         <v>17.4394509792753</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="16">
         <v>82</v>
       </c>
@@ -5252,8 +5355,11 @@
       <c r="F84" s="20">
         <v>12.1997</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="16">
         <v>83</v>
       </c>
@@ -5272,8 +5378,11 @@
       <c r="F85" s="20">
         <v>18.87821434</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="16">
         <v>84</v>
       </c>
@@ -5293,7 +5402,7 @@
         <v>15.8388161077538</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="16">
         <v>85</v>
       </c>
@@ -5313,7 +5422,7 @@
         <v>15.8388161077538</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="16">
         <v>86</v>
       </c>
@@ -5332,8 +5441,11 @@
       <c r="F88" s="20">
         <v>14.796045461746999</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="16">
         <v>87</v>
       </c>
@@ -5352,8 +5464,11 @@
       <c r="F89" s="20">
         <v>18.201387</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="16">
         <v>88</v>
       </c>
@@ -5373,7 +5488,7 @@
         <v>16.603845216441702</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="16">
         <v>89</v>
       </c>
@@ -5393,7 +5508,7 @@
         <v>16.923048917433899</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="16">
         <v>90</v>
       </c>
@@ -5412,8 +5527,11 @@
       <c r="F92" s="20">
         <v>15.0512932599002</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="16">
         <v>91</v>
       </c>
@@ -5432,8 +5550,11 @@
       <c r="F93" s="16">
         <v>15.427434598749</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="16">
         <v>92</v>
       </c>
@@ -5452,8 +5573,11 @@
       <c r="F94" s="20">
         <v>10.695925712585399</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="16">
         <v>93</v>
       </c>
@@ -5472,8 +5596,11 @@
       <c r="F95" s="20">
         <v>15.86863089</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="16">
         <v>94</v>
       </c>
@@ -5492,8 +5619,11 @@
       <c r="F96" s="20">
         <v>15.691419808344399</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="16">
         <v>95</v>
       </c>
@@ -5512,9 +5642,12 @@
       <c r="F97" s="17">
         <v>16.079637613094398</v>
       </c>
+      <c r="G97" s="25" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G97">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G97">
     <sortCondition descending="1" ref="E2:E102"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>